<commit_message>
add tests for load_results_Tecan
</commit_message>
<xml_diff>
--- a/inst/extdata/data2/manifest_Tecan_96_well_plates.xlsx
+++ b/inst/extdata/data2/manifest_Tecan_96_well_plates.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/datashare/files_rosalind/unit_test_gDRimport/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gerosal/gstore/home/gerosal/projects/work/gDRcode_2022_05/gDRimport/inst/extdata/data2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F17A8A2E-3C5E-604E-B841-C6295519F4D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B146F9E-BB0D-5C4F-95F8-C63B62A4C6D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5660" yWindow="3860" windowWidth="28040" windowHeight="17440" xr2:uid="{CFA3D1EC-9BB9-DC4D-8BF5-29E154E8E7C3}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
   <si>
     <t>Template</t>
   </si>
@@ -33,9 +33,6 @@
     <t>Duration</t>
   </si>
   <si>
-    <t>Plate</t>
-  </si>
-  <si>
     <t>clid</t>
   </si>
   <si>
@@ -51,7 +48,16 @@
     <t>CL130148</t>
   </si>
   <si>
-    <t>D300_trt_Tecan_96_well_plates</t>
+    <t>H358-2</t>
+  </si>
+  <si>
+    <t>H2122-2</t>
+  </si>
+  <si>
+    <t>Barcode</t>
+  </si>
+  <si>
+    <t>D300_trt_Tecan_96_well_plates.xlsx</t>
   </si>
 </sst>
 </file>
@@ -413,19 +419,19 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.1640625" customWidth="1"/>
     <col min="2" max="2" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -434,65 +440,65 @@
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2">
         <v>168</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B3">
         <v>168</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4">
         <v>168</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B5">
         <v>168</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>